<commit_message>
Checked in New Code
Checked in New Code
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/CallingModule/RegressionTestSuite.xlsx
+++ b/frameworkDemo/src/test/resources/CallingModule/RegressionTestSuite.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse-workspace\frameworkDemo\src\test\resources\CallingModule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\CallingModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113536B2-37C8-4782-B77E-DD0808BBBFC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63DB656-D5F5-465A-9E88-997807CF1376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{A0A3F6EA-F008-46B9-989F-9FD20058E9F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0A3F6EA-F008-46B9-989F-9FD20058E9F2}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -96,16 +96,34 @@
   </si>
   <si>
     <t>TC_Exel_004</t>
+  </si>
+  <si>
+    <t>TC_Exel_005</t>
+  </si>
+  <si>
+    <t>TC_Exel_006</t>
+  </si>
+  <si>
+    <t>TC_Exel_007</t>
+  </si>
+  <si>
+    <t>TC_Exel_008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -148,26 +166,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,23 +488,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2248757D-BC67-4CD5-A94D-615B987EA961}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -544,7 +550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -567,7 +573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -590,53 +596,146 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated TC in GIT
Updated TC in GIT
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/CallingModule/RegressionTestSuite.xlsx
+++ b/frameworkDemo/src/test/resources/CallingModule/RegressionTestSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\CallingModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63DB656-D5F5-465A-9E88-997807CF1376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB97E624-32EA-44F2-AA67-3FD527D8D153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0A3F6EA-F008-46B9-989F-9FD20058E9F2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>TC_Exel_008</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +550,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -570,7 +573,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -593,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -639,7 +642,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -662,7 +665,7 @@
         <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -685,7 +688,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -708,7 +711,7 @@
         <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -731,7 +734,7 @@
         <v>24</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Parameterization & Updated the Function for performance issue
Added Parameterization & Updated the Function for performance issue
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/CallingModule/RegressionTestSuite.xlsx
+++ b/frameworkDemo/src/test/resources/CallingModule/RegressionTestSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\CallingModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB97E624-32EA-44F2-AA67-3FD527D8D153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A15A60-9672-4DBA-9EC9-CA0311D03FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0A3F6EA-F008-46B9-989F-9FD20058E9F2}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Excel Input, Chatbot Chrome, SharpRunner
Updated Excel Input, Chatbot Chrome, SharpRunner
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/CallingModule/RegressionTestSuite.xlsx
+++ b/frameworkDemo/src/test/resources/CallingModule/RegressionTestSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\CallingModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A15A60-9672-4DBA-9EC9-CA0311D03FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC481B4-A363-4542-84B0-21E4127044CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0A3F6EA-F008-46B9-989F-9FD20058E9F2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="68">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -111,6 +111,132 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>TC_Exel_009</t>
+  </si>
+  <si>
+    <t>TC_Exel_010</t>
+  </si>
+  <si>
+    <t>TC_Exel_011</t>
+  </si>
+  <si>
+    <t>TC_Exel_012</t>
+  </si>
+  <si>
+    <t>TC_Exel_013</t>
+  </si>
+  <si>
+    <t>TC_Exel_014</t>
+  </si>
+  <si>
+    <t>TC_Exel_015</t>
+  </si>
+  <si>
+    <t>TC_Exel_016</t>
+  </si>
+  <si>
+    <t>TC_Exel_017</t>
+  </si>
+  <si>
+    <t>TC_Exel_018</t>
+  </si>
+  <si>
+    <t>TC_Exel_019</t>
+  </si>
+  <si>
+    <t>TC_Exel_020</t>
+  </si>
+  <si>
+    <t>TC_Exel_021</t>
+  </si>
+  <si>
+    <t>TC_Exel_022</t>
+  </si>
+  <si>
+    <t>TC_Exel_023</t>
+  </si>
+  <si>
+    <t>TC_Exel_024</t>
+  </si>
+  <si>
+    <t>TC_Exel_025</t>
+  </si>
+  <si>
+    <t>TC_Exel_026</t>
+  </si>
+  <si>
+    <t>TC_Exel_027</t>
+  </si>
+  <si>
+    <t>TC_Exel_028</t>
+  </si>
+  <si>
+    <t>TC_Exel_029</t>
+  </si>
+  <si>
+    <t>TC_Exel_030</t>
+  </si>
+  <si>
+    <t>TC_Exel_031</t>
+  </si>
+  <si>
+    <t>TC_Exel_032</t>
+  </si>
+  <si>
+    <t>TC_Exel_033</t>
+  </si>
+  <si>
+    <t>TC_Exel_034</t>
+  </si>
+  <si>
+    <t>TC_Exel_035</t>
+  </si>
+  <si>
+    <t>TC_Exel_036</t>
+  </si>
+  <si>
+    <t>TC_Exel_037</t>
+  </si>
+  <si>
+    <t>TC_Exel_038</t>
+  </si>
+  <si>
+    <t>TC_Exel_039</t>
+  </si>
+  <si>
+    <t>TC_Exel_040</t>
+  </si>
+  <si>
+    <t>TC_Exel_041</t>
+  </si>
+  <si>
+    <t>TC_Exel_042</t>
+  </si>
+  <si>
+    <t>TC_Exel_043</t>
+  </si>
+  <si>
+    <t>TC_Exel_044</t>
+  </si>
+  <si>
+    <t>TC_Exel_045</t>
+  </si>
+  <si>
+    <t>TC_Exel_046</t>
+  </si>
+  <si>
+    <t>TC_Exel_047</t>
+  </si>
+  <si>
+    <t>TC_Exel_048</t>
+  </si>
+  <si>
+    <t>TC_Exel_049</t>
+  </si>
+  <si>
+    <t>TC_Exel_050</t>
   </si>
 </sst>
 </file>
@@ -491,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2248757D-BC67-4CD5-A94D-615B987EA961}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -737,8 +863,979 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G52" xr:uid="{CCB81F6A-38D7-46FD-849C-A148F1879BD4}">
+      <formula1>"Y, N"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>